<commit_message>
fixed email app, now reads from excel file
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -27,19 +27,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>synergisticitsessionusc6@gmail.com</t>
   </si>
   <si>
     <t>session6</t>
   </si>
+  <si>
+    <t>triminhtran2797@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,6 +54,14 @@
       <sz val="13"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,14 +81,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,7 +383,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>